<commit_message>
Analysis of Audience cards
</commit_message>
<xml_diff>
--- a/analysis/Audience_Cards_List.xlsx
+++ b/analysis/Audience_Cards_List.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$46</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
   <si>
     <t>Audience Expectation</t>
   </si>
@@ -28,6 +30,9 @@
     <t>Decrease</t>
   </si>
   <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t>The crowd needs more alcohol stalls to keep the spirits up!</t>
   </si>
   <si>
@@ -58,7 +63,7 @@
     <t>We need more action figure stalls! Crows loves collectibles.</t>
   </si>
   <si>
-    <t>Merch Tshirts are far less! Bring in more to meet the demand.</t>
+    <t>Merch Tshirts are far less! Bring in more of those and decrease action figure stalls..</t>
   </si>
   <si>
     <t>We don't need more food stalls. We need more lounge areas!</t>
@@ -115,24 +120,27 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>Too much emphasis on Gold and Premium! Balance it with VIP.</t>
+    <t>Too much emphasis on Gold and Premium! Let's not bring anymore of these Lounge areas.</t>
+  </si>
+  <si>
+    <t>Gold, Premium</t>
+  </si>
+  <si>
+    <t>Modify</t>
+  </si>
+  <si>
+    <t>The Gold Lounges are almost empty. Why not focus more on VIP and Premium?</t>
+  </si>
+  <si>
+    <t>VIP, Premium</t>
+  </si>
+  <si>
+    <t>We need more VIP Lounges! The guests are feeling neglected.</t>
   </si>
   <si>
     <t>VIP</t>
   </si>
   <si>
-    <t>Gold, Premium</t>
-  </si>
-  <si>
-    <t>The Gold Lounges are almost empty. Why not focus more on VIP and Premium?</t>
-  </si>
-  <si>
-    <t>VIP, Premium</t>
-  </si>
-  <si>
-    <t>We need more VIP Lounges! The guests are feeling neglected.</t>
-  </si>
-  <si>
     <t>The crowd is thirsty! We need more soft-drink stalls.</t>
   </si>
   <si>
@@ -142,7 +150,7 @@
     <t>Too many soft-drinks around. Cut down the non-alcoholic stalls.</t>
   </si>
   <si>
-    <t>There is an overabundance of alcohol stalls. Tone it down!</t>
+    <t>There is an overabundance of alcohol stalls. Tone it down! Bring more soft drink stalls instead.</t>
   </si>
   <si>
     <t>A balanced line-up is the key! Add more beverage stalls.</t>
@@ -154,127 +162,130 @@
     <t>Lebanese</t>
   </si>
   <si>
-    <t>More continental food stalls, please!</t>
+    <t>Less Premium Lounge areas, please!</t>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>We are overwhelmed by too many VIP and Gold Lounges. Can we have more Chinese food stalls instead?</t>
+  </si>
+  <si>
+    <t>Lounge, Food</t>
+  </si>
+  <si>
+    <t>VIP, Gold, Chinese</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>VIP, Gold</t>
+  </si>
+  <si>
+    <t>There are people misbehaving. Can we have less alcohol stalls and more soft drinks stalls?</t>
+  </si>
+  <si>
+    <t>Can we have more Merch cloth stalls and less Lounges please?</t>
+  </si>
+  <si>
+    <t>Merchandise, Lounge</t>
+  </si>
+  <si>
+    <t>Clothes, VIP, Gold, Premium</t>
+  </si>
+  <si>
+    <t>Too many VIP Lounges and Continental food stalls. Can we cut down both?</t>
+  </si>
+  <si>
+    <t>VIP, Chinese</t>
+  </si>
+  <si>
+    <t>VIP, Continental</t>
+  </si>
+  <si>
+    <t>We need more alcohol with an increase in Indial food stalls as well.</t>
+  </si>
+  <si>
+    <t>Food, Beverage</t>
+  </si>
+  <si>
+    <t>Alcohol, Indian</t>
+  </si>
+  <si>
+    <t>We need less soft drink stalls and fewer Merch cloth stalls.</t>
+  </si>
+  <si>
+    <t>Clothes, Soft drinks</t>
+  </si>
+  <si>
+    <t>Beverage stalls are taking unnecessary space, can we reduce them and add more food stalls?</t>
+  </si>
+  <si>
+    <t>Alcohol, Soft drinks, Continental, Indian, Lebanese, Chinese</t>
+  </si>
+  <si>
+    <t>Continental, Indian, Lebanese, Chinese</t>
+  </si>
+  <si>
+    <t>More Chinese food with Premium Lounge areas.</t>
+  </si>
+  <si>
+    <t>Chinese, Premium</t>
+  </si>
+  <si>
+    <t>Lounge areas need to grow! We want all types of lounges.</t>
+  </si>
+  <si>
+    <t>Can't we have more action figure stalls but decrease the number of alcohol stalls?</t>
+  </si>
+  <si>
+    <t>Alcohol, Action figure</t>
+  </si>
+  <si>
+    <t>Not enough Merch clothes and alcohol stalls. Can we fix that?</t>
+  </si>
+  <si>
+    <t>Clothes, Alcohol</t>
+  </si>
+  <si>
+    <t>Too many Indian, Lebanese and Continental food stalls, please reduce.</t>
+  </si>
+  <si>
+    <t>Continental, Indian, Lebanese</t>
+  </si>
+  <si>
+    <t>Too many soft drinks, not enough Merch clothes! Can we have a balance between these?</t>
+  </si>
+  <si>
+    <t>Soft drinks, Clothes</t>
+  </si>
+  <si>
+    <t>The VIP Lounges need to be removed; but we need more action figure stalls.</t>
+  </si>
+  <si>
+    <t>Lounge, Merchandise</t>
+  </si>
+  <si>
+    <t>VIP, Action figure</t>
+  </si>
+  <si>
+    <t>Too many Chinese stalls. Let's introduce some more Continental options.</t>
+  </si>
+  <si>
+    <t>Chinese, Continental</t>
   </si>
   <si>
     <t>Continental</t>
   </si>
   <si>
-    <t>We are overwhelmed by too many VIP and Gold Lounges. Can we have more Chinese food stalls instead?</t>
-  </si>
-  <si>
-    <t>Lounge, Food</t>
-  </si>
-  <si>
-    <t>VIP, Gold, Chinese</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>VIP, Gold</t>
-  </si>
-  <si>
-    <t>There are people misbehaving. Can we have less alcohol stalls and more soft drinks stalls?</t>
-  </si>
-  <si>
-    <t>Can we have more Merch cloth stalls and less Lounges please?</t>
-  </si>
-  <si>
-    <t>Merchandise, Lounge</t>
-  </si>
-  <si>
-    <t>Clothes, VIP, Gold, Premium</t>
-  </si>
-  <si>
-    <t>Too many VIP Lounges and Chinese food stalls. Can we cut down both?</t>
-  </si>
-  <si>
-    <t>VIP, Chinese</t>
-  </si>
-  <si>
-    <t>We need more alcohol with an increase in Indial food stalls as well.</t>
-  </si>
-  <si>
-    <t>Food, Beverage</t>
-  </si>
-  <si>
-    <t>Alcohol, Indian</t>
-  </si>
-  <si>
-    <t>We need less soft drink stalls and fewer Merch cloth stalls.</t>
-  </si>
-  <si>
-    <t>Clothes, Soft drinks</t>
-  </si>
-  <si>
-    <t>Beverage stalls are taking unnecessary space, can we reduce them and add more food stalls?</t>
-  </si>
-  <si>
-    <t>Alcohol, Soft drinks, Continental, Indian, Lebanese, Chinese</t>
-  </si>
-  <si>
-    <t>Continental, Indian, Lebanese, Chinese</t>
-  </si>
-  <si>
-    <t>More Chinese food with Premium Lounge areas.</t>
-  </si>
-  <si>
-    <t>Chinese, Premium</t>
-  </si>
-  <si>
-    <t>Lounge areas need to grow! We want all types of lounges.</t>
-  </si>
-  <si>
-    <t>Can't we have more action figure stalls but decrease the number of alcohol stalls?</t>
-  </si>
-  <si>
-    <t>Alcohol, Action figure</t>
-  </si>
-  <si>
-    <t>Not enough Merch clothes and alcohol stalls. Can we fix that?</t>
-  </si>
-  <si>
-    <t>Clothes, Alcohol</t>
-  </si>
-  <si>
-    <t>Too many food stalls, but too less Lounge areas for sitting are available.</t>
-  </si>
-  <si>
-    <t>Continental, Indian, Lebanese, Chinese, VIP, Gold, Premium</t>
-  </si>
-  <si>
-    <t>Too many soft drinks, not enough Merch clothes! Can we have a balance between these?</t>
-  </si>
-  <si>
-    <t>Soft drinks, Clothes</t>
-  </si>
-  <si>
-    <t>The VIP Lounges need to be removed; but we need more action figure stalls.</t>
-  </si>
-  <si>
-    <t>Lounge, Merchandise</t>
-  </si>
-  <si>
-    <t>VIP, Action figure</t>
-  </si>
-  <si>
-    <t>Too many Chinese stalls. Let's introduce some more Continental options.</t>
-  </si>
-  <si>
-    <t>Chinese, Continental</t>
-  </si>
-  <si>
     <t>We need balanced food offerings. There are far too many Lebanese and Chinese stalls right now.</t>
   </si>
   <si>
     <t>Lebanese, Chinese</t>
   </si>
   <si>
-    <t>Add more continental and Lebanese food offerings.</t>
-  </si>
-  <si>
-    <t>Continental, Lebanese</t>
+    <t>Add more Lebanese food offerings.</t>
   </si>
   <si>
     <t>Let's bring more Continental and Indian food. Can you make that happen?</t>
@@ -299,6 +310,27 @@
   </si>
   <si>
     <t>Chinese food stalls are everywhere! it's overwhelming, cut back a little!</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Let's have more Gold Lounge areas for Audience comfort. There is lots of unused Premium Lounges, cut back on those.</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Add more Indian and Chinese food offerings.</t>
+  </si>
+  <si>
+    <t>Chinese, Indian</t>
+  </si>
+  <si>
+    <t>Too many Merch stalls are making the area overcrowded! Reduce them.</t>
+  </si>
+  <si>
+    <t>Bring more Merch stalls. Crowd is crazy about those!</t>
   </si>
 </sst>
 </file>
@@ -318,15 +350,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border/>
     <border>
       <left style="thin">
@@ -459,10 +503,94 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFB6D7A8"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFB6D7A8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB6D7A8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB6D7A8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB6D7A8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB6D7A8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB6D7A8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF93C47D"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF93C47D"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF93C47D"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF93C47D"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF93C47D"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF93C47D"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF93C47D"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF93C47D"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF93C47D"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF93C47D"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB6D7A8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB6D7A8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB6D7A8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB6D7A8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB6D7A8"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -470,13 +598,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFB6D7A8"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFB6D7A8"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFB6D7A8"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -500,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -537,16 +665,52 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="12" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="15" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="18" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -607,13 +771,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E42" displayName="Event_tasks1" name="Event_tasks1" id="1">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F46" displayName="Event_tasks1" name="Event_tasks1" id="1">
+  <autoFilter ref="$A$1:$F$46"/>
+  <tableColumns count="6">
     <tableColumn name="Audience Expectation" id="1"/>
     <tableColumn name="Attraction Category" id="2"/>
     <tableColumn name="Sub category" id="3"/>
     <tableColumn name="Increase" id="4"/>
     <tableColumn name="Decrease" id="5"/>
+    <tableColumn name="Note" id="6"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -829,6 +995,7 @@
     <col customWidth="1" min="1" max="1" width="59.13"/>
     <col customWidth="1" min="2" max="2" width="30.13"/>
     <col customWidth="1" min="3" max="5" width="35.38"/>
+    <col customWidth="1" min="8" max="8" width="15.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -844,661 +1011,995 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="11"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="7"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="E7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="11"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="C12" s="19" t="s">
         <v>36</v>
       </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>33</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="11"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="E16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11" t="s">
-        <v>7</v>
-      </c>
+      <c r="E17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>50</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>53</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="11"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>7</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="7"/>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>31</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="11"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A24" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="11"/>
+        <v>65</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="E26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>24</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="11"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>7</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="7"/>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="11"/>
+        <v>77</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="A32" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="16"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="16"/>
+      <c r="X32" s="16"/>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>41</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>35</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>52</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="E36" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="E36" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
     </row>
     <row r="37">
-      <c r="A37" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="11"/>
+      <c r="A37" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="14"/>
+      <c r="F37" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="16"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="16"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D39" s="10"/>
-      <c r="E39" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="E39" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="11"/>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>93</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" s="7"/>
     </row>
     <row r="41">
       <c r="A41" s="8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="11"/>
+        <v>96</v>
+      </c>
+      <c r="E41" s="10"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D42" s="14"/>
-      <c r="E42" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="E42" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="16"/>
+      <c r="X42" s="16"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
+      <c r="W44" s="16"/>
+      <c r="X44" s="16"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="16"/>
+      <c r="W45" s="16"/>
+      <c r="X45" s="16"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="16"/>
+      <c r="W46" s="16"/>
+      <c r="X46" s="16"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C2:E42">
+    <dataValidation type="list" allowBlank="1" sqref="C2:E46">
       <formula1>"Continental,Indian,Lebanese,Chinese,Alcohol,Soft drinks,Clothes,Action figure,VIP,Gold,Premium"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B42">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B46">
       <formula1>"Food,Beverage,Merchandise,Lounge"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>